<commit_message>
Updated BC workspace unit test after transformer addition
</commit_message>
<xml_diff>
--- a/FME_files/UNIT_TESTS/BC_FGP_XML_BUILDER_PROD_04/met/P-T_ETL_LOOKUP_TABLES.xlsx
+++ b/FME_files/UNIT_TESTS/BC_FGP_XML_BUILDER_PROD_04/met/P-T_ETL_LOOKUP_TABLES.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2505" yWindow="4680" windowWidth="31440" windowHeight="21000" tabRatio="868" firstSheet="40" activeTab="49"/>
+    <workbookView xWindow="2505" yWindow="4680" windowWidth="31440" windowHeight="21000" tabRatio="868" firstSheet="17" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="Codespace" sheetId="12" r:id="rId1"/>
@@ -30,43 +30,47 @@
     <sheet name="Format_TBS_QC" sheetId="28" r:id="rId16"/>
     <sheet name="FrenchTranslation" sheetId="8" r:id="rId17"/>
     <sheet name="Geohub_ON_URL" sheetId="52" r:id="rId18"/>
-    <sheet name="Geospatial_BC" sheetId="25" r:id="rId19"/>
-    <sheet name="Geospatial_QC_to_delete" sheetId="20" r:id="rId20"/>
-    <sheet name="Geospatial_ON_to_delete" sheetId="53" r:id="rId21"/>
-    <sheet name="GeospatialValidation" sheetId="63" r:id="rId22"/>
-    <sheet name="Keyword" sheetId="5" r:id="rId23"/>
-    <sheet name="License_QC" sheetId="27" r:id="rId24"/>
-    <sheet name="License_ON" sheetId="64" r:id="rId25"/>
-    <sheet name="NB_ESRISERVICES" sheetId="51" r:id="rId26"/>
-    <sheet name="NB_Keywords" sheetId="60" r:id="rId27"/>
-    <sheet name="NB_Remove" sheetId="46" r:id="rId28"/>
-    <sheet name="NB_GeoDataTypes" sheetId="55" r:id="rId29"/>
-    <sheet name="NB_SlashCountSeparator" sheetId="42" r:id="rId30"/>
-    <sheet name="NB_TOPICS_DATASET" sheetId="56" r:id="rId31"/>
-    <sheet name="NB_TOPICS_GENERIC" sheetId="57" r:id="rId32"/>
-    <sheet name="NB_LINKBUILDER_GEO" sheetId="58" r:id="rId33"/>
-    <sheet name="NB_LINKBUILDER_NONGEO" sheetId="59" r:id="rId34"/>
-    <sheet name="Progress" sheetId="10" r:id="rId35"/>
-    <sheet name="PyCSW_config" sheetId="40" r:id="rId36"/>
-    <sheet name="QC_JSON_CONFIG" sheetId="31" r:id="rId37"/>
-    <sheet name="QC_MAP_RES_REMOVE" sheetId="39" r:id="rId38"/>
-    <sheet name="ResourceType_TBS_QC" sheetId="32" r:id="rId39"/>
-    <sheet name="Role" sheetId="11" r:id="rId40"/>
-    <sheet name="Sector_NB" sheetId="43" r:id="rId41"/>
-    <sheet name="Sector_QC" sheetId="22" r:id="rId42"/>
-    <sheet name="SpatialRef" sheetId="13" r:id="rId43"/>
-    <sheet name="SpatialRepresentation" sheetId="14" r:id="rId44"/>
-    <sheet name="SubjectNTopic_TBS_QC" sheetId="30" r:id="rId45"/>
-    <sheet name="TransferLang_ON" sheetId="66" r:id="rId46"/>
-    <sheet name="UnmappedGeoData_ON" sheetId="61" r:id="rId47"/>
-    <sheet name="Update" sheetId="6" r:id="rId48"/>
-    <sheet name="UpdateFrequency_TBS_QC" sheetId="29" r:id="rId49"/>
-    <sheet name="UUID_Spatial_BC" sheetId="26" r:id="rId50"/>
-    <sheet name="UUID_Spatial_ON" sheetId="62" r:id="rId51"/>
-    <sheet name="UUID_Spatial_QC" sheetId="24" r:id="rId52"/>
-    <sheet name="ValidFormatList" sheetId="65" r:id="rId53"/>
-    <sheet name="WMS_URL_QC" sheetId="38" r:id="rId54"/>
+    <sheet name="GeoportalWeblink_BC" sheetId="67" r:id="rId19"/>
+    <sheet name="Geospatial_BC" sheetId="25" r:id="rId20"/>
+    <sheet name="Geospatial_QC_to_delete" sheetId="20" r:id="rId21"/>
+    <sheet name="Geospatial_ON_to_delete" sheetId="53" r:id="rId22"/>
+    <sheet name="GeospatialValidation" sheetId="63" r:id="rId23"/>
+    <sheet name="Keyword" sheetId="5" r:id="rId24"/>
+    <sheet name="License_QC" sheetId="27" r:id="rId25"/>
+    <sheet name="License_ON" sheetId="64" r:id="rId26"/>
+    <sheet name="NB_ESRISERVICES" sheetId="51" r:id="rId27"/>
+    <sheet name="NB_Keywords" sheetId="60" r:id="rId28"/>
+    <sheet name="NB_Remove" sheetId="46" r:id="rId29"/>
+    <sheet name="NB_GeoDataTypes" sheetId="55" r:id="rId30"/>
+    <sheet name="NB_SlashCountSeparator" sheetId="42" r:id="rId31"/>
+    <sheet name="NB_TOPICS_DATASET" sheetId="56" r:id="rId32"/>
+    <sheet name="NB_TOPICS_GENERIC" sheetId="57" r:id="rId33"/>
+    <sheet name="NB_LINKBUILDER_GEO" sheetId="58" r:id="rId34"/>
+    <sheet name="NB_LINKBUILDER_NONGEO" sheetId="59" r:id="rId35"/>
+    <sheet name="Progress" sheetId="10" r:id="rId36"/>
+    <sheet name="PyCSW_config" sheetId="40" r:id="rId37"/>
+    <sheet name="QC_JSON_CONFIG" sheetId="31" r:id="rId38"/>
+    <sheet name="QC_MAP_RES_REMOVE" sheetId="39" r:id="rId39"/>
+    <sheet name="ResourceType_TBS_QC" sheetId="32" r:id="rId40"/>
+    <sheet name="Role" sheetId="11" r:id="rId41"/>
+    <sheet name="Sector_NB" sheetId="43" r:id="rId42"/>
+    <sheet name="Sector_QC" sheetId="22" r:id="rId43"/>
+    <sheet name="SpatialRef" sheetId="13" r:id="rId44"/>
+    <sheet name="SpatialRepresentation" sheetId="14" r:id="rId45"/>
+    <sheet name="SubjectNTopic_TBS_QC" sheetId="30" r:id="rId46"/>
+    <sheet name="TransferLang_ON" sheetId="66" r:id="rId47"/>
+    <sheet name="UnmappedGeoData_ON" sheetId="61" r:id="rId48"/>
+    <sheet name="Update" sheetId="6" r:id="rId49"/>
+    <sheet name="UpdateFrequency_TBS_QC" sheetId="29" r:id="rId50"/>
+    <sheet name="UUID_Spatial_BC" sheetId="26" r:id="rId51"/>
+    <sheet name="UUID_Spatial_ON" sheetId="62" r:id="rId52"/>
+    <sheet name="UUID_Spatial_QC" sheetId="24" r:id="rId53"/>
+    <sheet name="ValidFormatList" sheetId="65" r:id="rId54"/>
+    <sheet name="WMS_URL_QC" sheetId="38" r:id="rId55"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Titles" localSheetId="18">GeoportalWeblink_BC!$1:$1</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -77,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7466" uniqueCount="2714">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7485" uniqueCount="2725">
   <si>
     <t>default_key</t>
   </si>
@@ -8224,6 +8228,39 @@
   </si>
   <si>
     <t>** Cet élément de métadonnées provenant d’une tierce partie. Les valeurs françaises pour le titre et la description du jeu de données proviennent de la province de l’Ontario alors que celles des mots-clés et des noms des ressources sont le résultat d'une traduction automatique (Amazon Translate) **</t>
+  </si>
+  <si>
+    <t>resources_format</t>
+  </si>
+  <si>
+    <t>resources_format_resourceType_en</t>
+  </si>
+  <si>
+    <t>resources_format_resourceType_fr</t>
+  </si>
+  <si>
+    <t>resources_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> British Columbia Geoportal</t>
+  </si>
+  <si>
+    <t>resources_protocol</t>
+  </si>
+  <si>
+    <t>resources_transfer_option_description_language</t>
+  </si>
+  <si>
+    <t>resources_transfer_option_description_language_other_lang</t>
+  </si>
+  <si>
+    <t>resources_url</t>
+  </si>
+  <si>
+    <t>https://catalogue.data.gov.bc.ca/dataset</t>
+  </si>
+  <si>
+    <t>resources_xlink_role</t>
   </si>
 </sst>
 </file>
@@ -18771,176 +18808,98 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.140625" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" customWidth="1"/>
+    <col min="1" max="1" width="72.7109375" customWidth="1"/>
+    <col min="2" max="2" width="48.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>962</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>864</v>
-      </c>
-      <c r="C1" t="s">
-        <v>965</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>886</v>
+        <v>2714</v>
       </c>
       <c r="B2" t="s">
-        <v>274</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1041</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>886</v>
+        <v>2715</v>
       </c>
       <c r="B3" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>886</v>
+        <v>2716</v>
       </c>
       <c r="B4" t="s">
-        <v>284</v>
-      </c>
-      <c r="C4" t="s">
-        <v>1027</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>883</v>
+        <v>2717</v>
       </c>
       <c r="B5" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2718</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>886</v>
+        <v>2719</v>
       </c>
       <c r="B6" t="s">
-        <v>294</v>
-      </c>
-      <c r="C6" t="s">
-        <v>1027</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>886</v>
+        <v>2720</v>
       </c>
       <c r="B7" t="s">
-        <v>296</v>
-      </c>
-      <c r="C7" t="s">
-        <v>1027</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2558</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>883</v>
+        <v>2721</v>
       </c>
       <c r="B8" t="s">
-        <v>781</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2560</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>883</v>
+        <v>2722</v>
       </c>
       <c r="B9" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2723</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>886</v>
-      </c>
-      <c r="B10" t="s">
-        <v>308</v>
-      </c>
-      <c r="C10" t="s">
-        <v>1027</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>883</v>
-      </c>
-      <c r="B11" t="s">
-        <v>311</v>
-      </c>
-      <c r="C11" t="s">
-        <v>1041</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>883</v>
-      </c>
-      <c r="B12" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>886</v>
-      </c>
-      <c r="B13" t="s">
-        <v>316</v>
-      </c>
-      <c r="C13" t="s">
-        <v>1041</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>886</v>
-      </c>
-      <c r="B14" t="s">
-        <v>318</v>
-      </c>
-      <c r="C14" t="s">
-        <v>1041</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>883</v>
-      </c>
-      <c r="B15" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>883</v>
-      </c>
-      <c r="B16" t="s">
-        <v>321</v>
+        <v>2724</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -19923,6 +19882,181 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.140625" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>962</v>
+      </c>
+      <c r="B1" t="s">
+        <v>864</v>
+      </c>
+      <c r="C1" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>886</v>
+      </c>
+      <c r="B2" t="s">
+        <v>274</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>886</v>
+      </c>
+      <c r="B3" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>886</v>
+      </c>
+      <c r="B4" t="s">
+        <v>284</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>883</v>
+      </c>
+      <c r="B5" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>886</v>
+      </c>
+      <c r="B6" t="s">
+        <v>294</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>886</v>
+      </c>
+      <c r="B7" t="s">
+        <v>296</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>883</v>
+      </c>
+      <c r="B8" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>883</v>
+      </c>
+      <c r="B9" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>886</v>
+      </c>
+      <c r="B10" t="s">
+        <v>308</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>883</v>
+      </c>
+      <c r="B11" t="s">
+        <v>311</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>883</v>
+      </c>
+      <c r="B12" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>886</v>
+      </c>
+      <c r="B13" t="s">
+        <v>316</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>886</v>
+      </c>
+      <c r="B14" t="s">
+        <v>318</v>
+      </c>
+      <c r="C14" t="s">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>883</v>
+      </c>
+      <c r="B15" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>883</v>
+      </c>
+      <c r="B16" t="s">
+        <v>321</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -20641,7 +20775,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C24"/>
   <sheetViews>
@@ -20892,7 +21026,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C68"/>
   <sheetViews>
@@ -21586,7 +21720,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B25"/>
   <sheetViews>
@@ -21804,7 +21938,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
@@ -21895,7 +22029,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B10"/>
   <sheetViews>
@@ -21994,7 +22128,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
@@ -22210,7 +22344,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B185"/>
   <sheetViews>
@@ -23712,7 +23846,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -23755,64 +23889,6 @@
       </c>
       <c r="B4" s="29" t="s">
         <v>1638</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="16384" width="10.85546875" style="37"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
-        <v>1839</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="37" t="s">
-        <v>1838</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="37" t="s">
-        <v>1837</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="37" t="s">
-        <v>1836</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="37" t="s">
-        <v>1835</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="37" t="s">
-        <v>1834</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="37" t="s">
-        <v>1833</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="37" t="s">
-        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -24721,6 +24797,64 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="10.85546875" style="37"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="37" t="s">
+        <v>1839</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="37" t="s">
+        <v>1838</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="37" t="s">
+        <v>1837</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="37" t="s">
+        <v>1836</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="37" t="s">
+        <v>1835</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="37" t="s">
+        <v>1834</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="37" t="s">
+        <v>1833</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="37" t="s">
+        <v>208</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -24763,7 +24897,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B76"/>
   <sheetViews>
@@ -25392,7 +25526,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B33"/>
   <sheetViews>
@@ -25676,7 +25810,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -25767,7 +25901,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
@@ -25900,7 +26034,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
@@ -26075,7 +26209,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -26160,7 +26294,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C44"/>
   <sheetViews>
@@ -26664,7 +26798,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A107"/>
   <sheetViews>
@@ -27218,69 +27352,6 @@
     <hyperlink ref="A9" r:id="rId2"/>
     <hyperlink ref="A15" r:id="rId3"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>1252</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1251</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1320</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1319</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1318</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1317</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>1316</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1230</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>1315</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1314</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1230</v>
-      </c>
-    </row>
-  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -28078,6 +28149,69 @@
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1252</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1251</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1320</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1319</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1318</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1316</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1315</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1314</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -28335,7 +28469,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C17"/>
   <sheetViews>
@@ -28540,7 +28674,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E77"/>
   <sheetViews>
@@ -29916,7 +30050,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B18"/>
   <sheetViews>
@@ -30081,7 +30215,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
@@ -30200,7 +30334,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C14"/>
   <sheetViews>
@@ -30374,7 +30508,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -30438,7 +30572,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B518"/>
   <sheetViews>
@@ -33745,7 +33879,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D35"/>
   <sheetViews>
@@ -34254,149 +34388,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>1252</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1251</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>856</v>
-      </c>
-      <c r="B2" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>857</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1263</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>243</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1262</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>224</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1261</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>240</v>
-      </c>
-      <c r="B6" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>858</v>
-      </c>
-      <c r="B7" t="s">
-        <v>1260</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>248</v>
-      </c>
-      <c r="B8" t="s">
-        <v>1259</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>859</v>
-      </c>
-      <c r="B9" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>234</v>
-      </c>
-      <c r="B10" t="s">
-        <v>1258</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>860</v>
-      </c>
-      <c r="B11" t="s">
-        <v>1257</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>861</v>
-      </c>
-      <c r="B12" t="s">
-        <v>1256</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>251</v>
-      </c>
-      <c r="B13" t="s">
-        <v>1255</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>260</v>
-      </c>
-      <c r="B14" t="s">
-        <v>1254</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>862</v>
-      </c>
-      <c r="B15" t="s">
-        <v>1253</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" t="s">
-        <v>24</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -35301,9 +35292,152 @@
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1252</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1251</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>856</v>
+      </c>
+      <c r="B2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>857</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1263</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>243</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1262</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>224</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>240</v>
+      </c>
+      <c r="B6" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>858</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1260</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>248</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1259</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>859</v>
+      </c>
+      <c r="B9" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>234</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>860</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1257</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>861</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1256</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>251</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>260</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1254</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>862</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1253</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A35" sqref="A35:XFD35"/>
     </sheetView>
   </sheetViews>
@@ -36433,7 +36567,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B84"/>
   <sheetViews>
@@ -37127,7 +37261,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B22"/>
   <sheetViews>
@@ -37325,7 +37459,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A116"/>
   <sheetViews>
@@ -37923,7 +38057,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C100"/>
   <sheetViews>

</xml_diff>